<commit_message>
Bracket preparation mechanism in progress.
</commit_message>
<xml_diff>
--- a/TRNMNT/DocSamples/FightersListSample.xlsx
+++ b/TRNMNT/DocSamples/FightersListSample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
   <si>
     <t>First Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Ribeiro JJ</t>
   </si>
   <si>
-    <t>Adult White</t>
-  </si>
-  <si>
     <t>Saulo</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Pena</t>
   </si>
   <si>
-    <t>Kids 1</t>
-  </si>
-  <si>
     <t>Andre</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>CTA</t>
   </si>
   <si>
-    <t>Adult Blue</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yan </t>
   </si>
   <si>
@@ -129,12 +120,6 @@
     <t>Checkmat</t>
   </si>
   <si>
-    <t>+100</t>
-  </si>
-  <si>
-    <t>-60</t>
-  </si>
-  <si>
     <t>Date Of Birth</t>
   </si>
   <si>
@@ -142,6 +127,132 @@
   </si>
   <si>
     <t>Rafael</t>
+  </si>
+  <si>
+    <t>Miao</t>
+  </si>
+  <si>
+    <t>Joao</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Malfacine</t>
+  </si>
+  <si>
+    <t>Paulo</t>
+  </si>
+  <si>
+    <t>Otavio</t>
+  </si>
+  <si>
+    <t>Sousa</t>
+  </si>
+  <si>
+    <t>Calasans</t>
+  </si>
+  <si>
+    <t>Claudio</t>
+  </si>
+  <si>
+    <t>Leandro</t>
+  </si>
+  <si>
+    <t>Lo</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Lepri</t>
+  </si>
+  <si>
+    <t>Fabio</t>
+  </si>
+  <si>
+    <t>Gurgel</t>
+  </si>
+  <si>
+    <t>Paiva</t>
+  </si>
+  <si>
+    <t>Alexandre</t>
+  </si>
+  <si>
+    <t>Ze</t>
+  </si>
+  <si>
+    <t>Radiola</t>
+  </si>
+  <si>
+    <t>Rocha</t>
+  </si>
+  <si>
+    <t>Rubens</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Artem</t>
+  </si>
+  <si>
+    <t>Sydorov</t>
+  </si>
+  <si>
+    <t>Vadim</t>
+  </si>
+  <si>
+    <t>Puzanov</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Silverio</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>Glover</t>
+  </si>
+  <si>
+    <t>Garry</t>
+  </si>
+  <si>
+    <t>Tonnon</t>
+  </si>
+  <si>
+    <t>Renzo</t>
+  </si>
+  <si>
+    <t>Gracie</t>
+  </si>
+  <si>
+    <t>Bernardo</t>
+  </si>
+  <si>
+    <t>Faria</t>
+  </si>
+  <si>
+    <t>Eberth</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Mendes</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -466,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -486,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -511,8 +622,8 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2">
-        <v>-90</v>
+      <c r="E2" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -535,12 +646,12 @@
         <v>90</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -555,144 +666,144 @@
         <v>90</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C5" s="4">
         <v>29924</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2">
-        <v>90</v>
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="4">
         <v>29925</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
-        <v>-40</v>
+        <v>90</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4">
         <v>29926</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4">
         <v>29927</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="4">
         <v>29928</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>-80</v>
+        <v>90</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="4">
         <v>29929</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>-100</v>
+        <v>90</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="4">
         <v>29930</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="E11" s="2">
+        <v>90</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -700,21 +811,461 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4">
         <v>29565</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4">
+        <v>29921</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>90</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4">
+        <v>29922</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <v>90</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="4">
+        <v>29923</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4">
+        <v>29924</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <v>90</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="4">
+        <v>29925</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2">
+        <v>90</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="4">
+        <v>29926</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2">
+        <v>90</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="4">
+        <v>29927</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2">
+        <v>90</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="4">
+        <v>29928</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="2">
+        <v>90</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="4">
+        <v>29929</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2">
+        <v>90</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="4">
+        <v>29930</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="2">
+        <v>90</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="4">
+        <v>29565</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="2">
+        <v>90</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="4">
+        <v>29921</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2">
+        <v>90</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="4">
+        <v>29922</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="2">
+        <v>90</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="4">
+        <v>29923</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="2">
+        <v>90</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="4">
+        <v>29924</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="2">
+        <v>90</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="4">
+        <v>29925</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="4">
+        <v>29926</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="4">
+        <v>29927</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2">
+        <v>90</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="4">
+        <v>29928</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="2">
+        <v>90</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="4">
+        <v>29929</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2">
+        <v>90</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="4">
+        <v>29930</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="2">
+        <v>90</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="2">
-        <v>-100</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="4">
+        <v>29565</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="2">
+        <v>90</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>